<commit_message>
Personnes + magasins suite
</commit_message>
<xml_diff>
--- a/ProjetJava1/avancement.xlsx
+++ b/ProjetJava1/avancement.xlsx
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -518,7 +518,7 @@
       <c r="B2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="1"/>
       <c r="D2" t="s">
         <v>39</v>
       </c>
@@ -530,7 +530,7 @@
       <c r="B3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -548,7 +548,7 @@
       <c r="B5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -557,7 +557,7 @@
       <c r="B6" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -566,7 +566,7 @@
       <c r="B7" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -575,7 +575,7 @@
       <c r="B8" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -584,7 +584,7 @@
       <c r="B9" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -593,7 +593,7 @@
       <c r="B10" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -602,7 +602,7 @@
       <c r="B11" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -611,7 +611,7 @@
       <c r="B12" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -620,7 +620,7 @@
       <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -629,7 +629,7 @@
       <c r="B14" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -638,7 +638,7 @@
       <c r="B15" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -647,7 +647,7 @@
       <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">

</xml_diff>